<commit_message>
add powershell solve two files, and get diff
</commit_message>
<xml_diff>
--- a/excel/test.xlsx
+++ b/excel/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code data\CMD\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50C7987C-C6BA-4316-BF73-116CCB2CC1B2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75A5C111-3F0B-4C4C-9F5F-5BD8A412D362}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3936" yWindow="1752" windowWidth="17280" windowHeight="8964" xr2:uid="{FF966766-96C8-4BD7-88C9-D5C576E9332E}"/>
+    <workbookView xWindow="3468" yWindow="1932" windowWidth="17280" windowHeight="8964" xr2:uid="{F154B77A-52F2-4B5A-B244-B78E62E38C8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -227,7 +227,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5229-4011-973D-238B069245CA}"/>
+              <c16:uniqueId val="{00000001-FEAC-4CE6-98D2-B09EEC56A24D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -241,11 +241,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="918304592"/>
-        <c:axId val="918894944"/>
+        <c:axId val="1424611696"/>
+        <c:axId val="1423386992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="918304592"/>
+        <c:axId val="1424611696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -255,7 +255,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="918894944"/>
+        <c:crossAx val="1423386992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -263,7 +263,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="918894944"/>
+        <c:axId val="1423386992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -274,7 +274,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="918304592"/>
+        <c:crossAx val="1424611696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -322,7 +322,7 @@
         <xdr:cNvPr id="2" name="图表 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0CBC0DF-EEA4-4579-8944-AC19BACF05F0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A91A539-6871-4D7B-BAB4-92FF4F15153D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -639,7 +639,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44477C00-FBA4-44D7-B430-3E7E9D74D8C1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884B4B53-C375-4E95-9183-990DC1B04DEE}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>